<commit_message>
made mediapipe model. Found frame mistake in app
</commit_message>
<xml_diff>
--- a/temp/markup.xlsx
+++ b/temp/markup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my_github\paresis_detection\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\my_github\paresis_detection\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3A6D71-58B2-4212-8C84-15AB6ADB05CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C424176A-D46E-4197-82A7-D0E168DA2040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2240" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="4185" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>eyebrows_raising_begin</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>20180125_Mordashov_1</t>
+  </si>
+  <si>
+    <t>rest_begin</t>
+  </si>
+  <si>
+    <t>rest_end</t>
   </si>
 </sst>
 </file>
@@ -449,141 +455,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>162</v>
+      </c>
+      <c r="D2">
         <v>393</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>439</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>169</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>209</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>210</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>255</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>259</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>311</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>469</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>503</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>515</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>605</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>693</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>742</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <v>625</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>680</v>
       </c>
-      <c r="R2">
+      <c r="T2">
         <v>765</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <v>807</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <v>866</v>
       </c>
-      <c r="U2">
+      <c r="W2">
         <v>923</v>
       </c>
     </row>

</xml_diff>